<commit_message>
Update Equitable Estate Distribution Formula.xlsx
</commit_message>
<xml_diff>
--- a/Equitable Estate Distribution Formula.xlsx
+++ b/Equitable Estate Distribution Formula.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylet\Documents\GitHub\equitable-distribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403F289C-C1CE-460D-981C-D04D90AB2D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAD2419-70C1-4926-BDEA-07754E00E2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C203B1D9-A441-4F76-A4FC-797AD900F99A}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{C203B1D9-A441-4F76-A4FC-797AD900F99A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{03514290-5DE0-43C3-B33D-C5FB74F15EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution Formula" sheetId="2" r:id="rId1"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Person</t>
   </si>
@@ -80,22 +81,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Adjusted Income</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Outlier Fix</t>
-  </si>
-  <si>
     <t>Money Given</t>
-  </si>
-  <si>
-    <t>Take people's income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adjust to bring distributions closer to ^1/x </t>
   </si>
   <si>
     <t>B</t>
@@ -110,25 +96,10 @@
     <t>F</t>
   </si>
   <si>
-    <t>Adjust to bring low outlier distributions within a range</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>Distribution of Estate</t>
   </si>
   <si>
-    <t>Proportion</t>
-  </si>
-  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Calculate proportions</t>
-  </si>
-  <si>
-    <t>Calculate percentages</t>
   </si>
   <si>
     <t>A</t>
@@ -141,9 +112,6 @@
   </si>
   <si>
     <t>INPUTS</t>
-  </si>
-  <si>
-    <t>Variation Level</t>
   </si>
   <si>
     <t>Estate Value</t>
@@ -178,6 +146,30 @@
   <si>
     <t>Parvati</t>
   </si>
+  <si>
+    <t>Fairness Adjustment</t>
+  </si>
+  <si>
+    <t>incomeShares</t>
+  </si>
+  <si>
+    <t>adjustedIncomeShares</t>
+  </si>
+  <si>
+    <t>normalizedShares</t>
+  </si>
+  <si>
+    <t>People's Income</t>
+  </si>
+  <si>
+    <t>Their share of the total income</t>
+  </si>
+  <si>
+    <t>Their equitable share of the total income. Reverse it and add the Fairness Adjustment</t>
+  </si>
+  <si>
+    <t>Normalize the equitable shares. Percentage of estate.</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +179,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +224,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,31 +262,37 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
     <dxf>
+      <font>
+        <b/>
+      </font>
       <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -308,22 +314,15 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
@@ -343,66 +342,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <font>
@@ -594,39 +534,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Distribution Formula'!$G$2:$G$11</c:f>
+              <c:f>'Distribution Formula'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10245.538910054063</c:v>
+                  <c:v>22569.660696283328</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25060.984838394023</c:v>
+                  <c:v>71692.481944865998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>172216.37536112618</c:v>
+                  <c:v>139884.32979851507</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60079.143719634492</c:v>
+                  <c:v>109916.29999932673</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>172216.37536112618</c:v>
+                  <c:v>144718.22813243122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>172216.37536112618</c:v>
+                  <c:v>137738.1017932781</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>172216.37536112618</c:v>
+                  <c:v>135196.23626836351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40970.486007211628</c:v>
+                  <c:v>95516.026145689277</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2561.9697190749703</c:v>
+                  <c:v>1.7179459537527544</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>172216.37536112618</c:v>
+                  <c:v>142766.917275293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,7 +758,438 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Distribution Formula'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Money Given</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Distribution Formula'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Harry</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hermione</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ron</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Neville</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Luna</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dean</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seamus</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cho</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Parvati</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Distribution Formula'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22569.660696283328</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71692.481944865998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139884.32979851507</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>109916.29999932673</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144718.22813243122</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137738.1017932781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135196.23626836351</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95516.026145689277</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7179459537527544</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>142766.917275293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1564-4FCD-B2E4-758003910859}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1374,20 +1745,539 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1227137</xdr:colOff>
+      <xdr:colOff>40264</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>17462</xdr:rowOff>
+      <xdr:rowOff>5917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>446087</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>353723</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:rowOff>42430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1412,29 +2302,62 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>212725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7175FF87-CC54-5A9D-3AF1-472CF81FC816}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71D1AE78-A15B-42D0-9A66-8EDA80DCC903}" name="Table13" displayName="Table13" ref="A1:G12" totalsRowCount="1">
-  <autoFilter ref="A1:G11" xr:uid="{9B3D1B1D-5576-400C-A112-08800841837B}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71D1AE78-A15B-42D0-9A66-8EDA80DCC903}" name="Table13" displayName="Table13" ref="A1:F12" totalsRowCount="1">
+  <autoFilter ref="A1:F11" xr:uid="{9B3D1B1D-5576-400C-A112-08800841837B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{341E2D25-143C-468D-A404-231DE4346564}" name="Person" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{1419DA39-DF8B-411E-95C3-4E3A8BC59938}" name="Yearly Income" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{A981B2B8-EE26-46F6-AB20-F8AB6B21DF5C}" name="Adjusted Income" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="4" dataCellStyle="Currency">
-      <calculatedColumnFormula>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{1419DA39-DF8B-411E-95C3-4E3A8BC59938}" name="Yearly Income" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{A981B2B8-EE26-46F6-AB20-F8AB6B21DF5C}" name="incomeShares" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="5" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{47EDF43E-22EB-413C-A13F-35E20DE37F72}" name="Outlier Fix" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Currency">
-      <calculatedColumnFormula>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{47EDF43E-22EB-413C-A13F-35E20DE37F72}" name="adjustedIncomeShares" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="4" dataCellStyle="Percent">
+      <calculatedColumnFormula>(1-Table13[[#This Row],[incomeShares]])^$B$16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{57A02392-FF7E-41A8-87F5-C5B1C426D82A}" name="Proportion" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Percent">
-      <calculatedColumnFormula>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{57A02392-FF7E-41A8-87F5-C5B1C426D82A}" name="normalizedShares" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{19BE0092-E16D-445F-8E73-924F9CA5658B}" name="Percentage" totalsRowFunction="sum" totalsRowDxfId="1">
-      <calculatedColumnFormula>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{F57C13EB-CBD1-44A8-93D6-F7217F99C514}" name="Money Given" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="0">
-      <calculatedColumnFormula>Table13[[#This Row],[Percentage]]*$B$17</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{F57C13EB-CBD1-44A8-93D6-F7217F99C514}" name="Money Given" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table13[[#This Row],[normalizedShares]]*$B$17</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1738,27 +2661,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D8AA85-0B98-470F-9CD3-2AAA3B7D5A81}">
-  <dimension ref="A1:J272"/>
+  <dimension ref="A1:I272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" workbookViewId="1">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1766,351 +2691,304 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>250000</v>
       </c>
-      <c r="C2" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>247808.7662665543</v>
-      </c>
-      <c r="D2" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>247808.7662665543</v>
+      <c r="C2" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>0.16957545090112394</v>
+      </c>
+      <c r="D2" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.155955894344076</v>
       </c>
       <c r="E2" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>6.1259773992836185E-2</v>
-      </c>
-      <c r="F2" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>1.0245538910054064E-2</v>
-      </c>
-      <c r="G2" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>10245.538910054063</v>
-      </c>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>2.2569660696283328E-2</v>
+      </c>
+      <c r="F2" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>22569.660696283328</v>
+      </c>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>100000</v>
       </c>
-      <c r="C3" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>101310.2387399703</v>
-      </c>
-      <c r="D3" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>101310.2387399703</v>
+      <c r="C3" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>6.7830180360449577E-2</v>
+      </c>
+      <c r="D3" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.49539358565985497</v>
       </c>
       <c r="E3" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>0.14984377890863049</v>
-      </c>
-      <c r="F3" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>2.5060984838394022E-2</v>
-      </c>
-      <c r="G3" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>25060.984838394023</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>7.1692481944865993E-2</v>
+      </c>
+      <c r="F3" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>71692.481944865998</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>5000</v>
       </c>
-      <c r="C4" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>7727.2705181092851</v>
-      </c>
-      <c r="D4" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>14742.7</v>
+      <c r="C4" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>3.3915090180224789E-3</v>
+      </c>
+      <c r="D4" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.96659786126255876</v>
       </c>
       <c r="E4" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.0297102304823869</v>
-      </c>
-      <c r="F4" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>0.17221637536112619</v>
-      </c>
-      <c r="G4" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>172216.37536112618</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.13988432979851506</v>
+      </c>
+      <c r="F4" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>139884.32979851507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>40000</v>
       </c>
-      <c r="C5" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>42259.829282598854</v>
-      </c>
-      <c r="D5" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>42259.829282598854</v>
+      <c r="C5" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>2.7132072144179831E-2</v>
+      </c>
+      <c r="D5" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.75951938755595227</v>
       </c>
       <c r="E5" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>0.35922315051053877</v>
-      </c>
-      <c r="F5" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>6.0079143719634492E-2</v>
-      </c>
-      <c r="G5" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>60079.143719634492</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.10991629999932673</v>
+      </c>
+      <c r="F5" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>109916.29999932673</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>2790.7312706968564</v>
-      </c>
-      <c r="D6" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>14742.7</v>
+      <c r="C6" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.0297102304823869</v>
-      </c>
-      <c r="F6" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>0.17221637536112619</v>
-      </c>
-      <c r="G6" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>172216.37536112618</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.14471822813243121</v>
+      </c>
+      <c r="F6" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>144718.22813243122</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>7270</v>
       </c>
-      <c r="C7" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>9968.2148533161635</v>
-      </c>
-      <c r="D7" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>14742.7</v>
+      <c r="C7" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>4.9312541122046843E-3</v>
+      </c>
+      <c r="D7" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.95176746959086855</v>
       </c>
       <c r="E7" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.0297102304823869</v>
-      </c>
-      <c r="F7" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>0.17221637536112619</v>
-      </c>
-      <c r="G7" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>172216.37536112618</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.13773810179327808</v>
+      </c>
+      <c r="F7" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>137738.1017932781</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>10000</v>
       </c>
-      <c r="C8" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>12663.062611940124</v>
-      </c>
-      <c r="D8" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>14742.7</v>
+      <c r="C8" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>6.7830180360449579E-3</v>
+      </c>
+      <c r="D8" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.93420323074053846</v>
       </c>
       <c r="E8" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.0297102304823869</v>
-      </c>
-      <c r="F8" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>0.17221637536112619</v>
-      </c>
-      <c r="G8" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>172216.37536112618</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.13519623626836352</v>
+      </c>
+      <c r="F8" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>135196.23626836351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>60000</v>
       </c>
-      <c r="C9" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>61969.8374236901</v>
-      </c>
-      <c r="D9" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>61969.8374236901</v>
+      <c r="C9" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>4.0698108216269749E-2</v>
+      </c>
+      <c r="D9" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.66001378940518018</v>
       </c>
       <c r="E9" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>0.24496932130290427</v>
-      </c>
-      <c r="F9" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>4.0970486007211628E-2</v>
-      </c>
-      <c r="G9" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>40970.486007211628</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>9.551602614568927E-2</v>
+      </c>
+      <c r="F9" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>95516.026145689277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1">
         <v>1000000</v>
       </c>
-      <c r="C10" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>991008.72978045477</v>
-      </c>
-      <c r="D10" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>991008.72978045477</v>
+      <c r="C10" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>0.67830180360449577</v>
+      </c>
+      <c r="D10" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>1.1870971445149725E-5</v>
       </c>
       <c r="E10" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.5318441259640341E-2</v>
-      </c>
-      <c r="F10" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>2.5619697190749705E-3</v>
-      </c>
-      <c r="G10" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>2561.9697190749703</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>1.7179459537527544E-6</v>
+      </c>
+      <c r="F10" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>1.7179459537527544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>2000</v>
       </c>
-      <c r="C11" s="1">
-        <f>IF(Table13[[#This Row],[Yearly Income]]&lt;Table13[[#Totals],[Yearly Income]], (Table13[[#This Row],[Yearly Income]]+((Table13[[#Totals],[Yearly Income]]-Table13[[#This Row],[Yearly Income]]))^(1/$B$16)),(Table13[[#This Row],[Yearly Income]]-((Table13[[#This Row],[Yearly Income]]-Table13[[#Totals],[Yearly Income]]))^(1/$B$16)))</f>
-        <v>4765.4344166240508</v>
-      </c>
-      <c r="D11" s="1">
-        <f>IF(Table13[[#This Row],[Adjusted Income]]&lt;(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),(Table13[[#Totals],[Yearly Income]]/COUNTA(Table13[Yearly Income])),Table13[[#This Row],[Adjusted Income]])</f>
-        <v>14742.7</v>
+      <c r="C11" s="11">
+        <f>Table13[[#This Row],[Yearly Income]]/SUM(Table13[Yearly Income])</f>
+        <v>1.3566036072089915E-3</v>
+      </c>
+      <c r="D11" s="11">
+        <f>(1-Table13[[#This Row],[incomeShares]])^$B$16</f>
+        <v>0.98651648183978213</v>
       </c>
       <c r="E11" s="4">
-        <f>1/(Table13[[#This Row],[Outlier Fix]]/Table13[[#Totals],[Outlier Fix]])/100</f>
-        <v>1.0297102304823869</v>
-      </c>
-      <c r="F11" s="9">
-        <f>Table13[[#This Row],[Proportion]]/Table13[[#Totals],[Proportion]]</f>
-        <v>0.17221637536112619</v>
-      </c>
-      <c r="G11" s="3">
-        <f>Table13[[#This Row],[Percentage]]*$B$17</f>
-        <v>172216.37536112618</v>
-      </c>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <f>Table13[[#This Row],[adjustedIncomeShares]]/(SUM(Table13[adjustedIncomeShares]))</f>
+        <v>0.142766917275293</v>
+      </c>
+      <c r="F11" s="13">
+        <f>Table13[[#This Row],[normalizedShares]]*$B$17</f>
+        <v>142766.917275293</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="3">
         <f>SUBTOTAL(101,Table13[Yearly Income])</f>
         <v>147427</v>
       </c>
-      <c r="C12" s="8">
-        <f>SUBTOTAL(109,Table13[Adjusted Income])</f>
-        <v>1482272.1151639547</v>
-      </c>
-      <c r="D12" s="8">
-        <f>SUBTOTAL(109,Table13[Outlier Fix])</f>
-        <v>1518070.9014932683</v>
-      </c>
-      <c r="E12" s="7">
-        <f>SUBTOTAL(109,Table13[Proportion])</f>
-        <v>5.9791656183864834</v>
-      </c>
-      <c r="F12" s="9">
-        <f>SUBTOTAL(109,Table13[Percentage])</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="C12" s="3">
+        <f>SUBTOTAL(109,Table13[incomeShares])</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f>SUBTOTAL(109,Table13[adjustedIncomeShares])</f>
+        <v>6.9099795713702568</v>
+      </c>
+      <c r="E12" s="6">
+        <f>SUBTOTAL(109,Table13[normalizedShares])</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="F12" s="14">
         <f>SUBTOTAL(109,Table13[Money Given])</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="13"/>
+    <row r="15" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>24</v>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
@@ -2118,7 +2996,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>1000000</v>
@@ -2170,10 +3048,9 @@
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
@@ -2236,10 +3113,9 @@
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="8"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
@@ -2302,10 +3178,9 @@
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="8"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="6"/>
+      <c r="E51" s="6"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
@@ -2368,10 +3243,9 @@
       <c r="E63" s="4"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B64" s="8"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="7"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="6"/>
+      <c r="E64" s="6"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
@@ -2434,10 +3308,9 @@
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="8"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="7"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="6"/>
+      <c r="E77" s="6"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
@@ -2500,10 +3373,9 @@
       <c r="E89" s="4"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B90" s="8"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="7"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="6"/>
+      <c r="E90" s="6"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B93" s="1"/>
@@ -2566,10 +3438,9 @@
       <c r="E102" s="4"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B103" s="8"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="7"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="6"/>
+      <c r="E103" s="6"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B106" s="1"/>
@@ -2632,10 +3503,9 @@
       <c r="E115" s="4"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B116" s="8"/>
-      <c r="C116" s="7"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="7"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="6"/>
+      <c r="E116" s="6"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B119" s="1"/>
@@ -2698,10 +3568,9 @@
       <c r="E128" s="4"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B129" s="8"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="7"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="6"/>
+      <c r="E129" s="6"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B132" s="1"/>
@@ -2764,10 +3633,9 @@
       <c r="E141" s="4"/>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B142" s="8"/>
-      <c r="C142" s="7"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="7"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="6"/>
+      <c r="E142" s="6"/>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B145" s="1"/>
@@ -2830,10 +3698,9 @@
       <c r="E154" s="4"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B155" s="8"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="6"/>
-      <c r="E155" s="7"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="6"/>
+      <c r="E155" s="6"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B158" s="1"/>
@@ -2896,10 +3763,9 @@
       <c r="E167" s="4"/>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B168" s="8"/>
-      <c r="C168" s="7"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="7"/>
+      <c r="B168" s="3"/>
+      <c r="C168" s="6"/>
+      <c r="E168" s="6"/>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B171" s="1"/>
@@ -2962,10 +3828,9 @@
       <c r="E180" s="4"/>
     </row>
     <row r="181" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B181" s="8"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="6"/>
-      <c r="E181" s="7"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="6"/>
+      <c r="E181" s="6"/>
     </row>
     <row r="184" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B184" s="1"/>
@@ -3028,10 +3893,9 @@
       <c r="E193" s="4"/>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B194" s="8"/>
-      <c r="C194" s="7"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="7"/>
+      <c r="B194" s="3"/>
+      <c r="C194" s="6"/>
+      <c r="E194" s="6"/>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B197" s="1"/>
@@ -3094,10 +3958,9 @@
       <c r="E206" s="4"/>
     </row>
     <row r="207" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B207" s="8"/>
-      <c r="C207" s="7"/>
-      <c r="D207" s="6"/>
-      <c r="E207" s="7"/>
+      <c r="B207" s="3"/>
+      <c r="C207" s="6"/>
+      <c r="E207" s="6"/>
     </row>
     <row r="210" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B210" s="1"/>
@@ -3160,10 +4023,9 @@
       <c r="E219" s="4"/>
     </row>
     <row r="220" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B220" s="8"/>
-      <c r="C220" s="7"/>
-      <c r="D220" s="6"/>
-      <c r="E220" s="7"/>
+      <c r="B220" s="3"/>
+      <c r="C220" s="6"/>
+      <c r="E220" s="6"/>
     </row>
     <row r="223" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B223" s="1"/>
@@ -3226,10 +4088,9 @@
       <c r="E232" s="4"/>
     </row>
     <row r="233" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B233" s="8"/>
-      <c r="C233" s="7"/>
-      <c r="D233" s="6"/>
-      <c r="E233" s="7"/>
+      <c r="B233" s="3"/>
+      <c r="C233" s="6"/>
+      <c r="E233" s="6"/>
     </row>
     <row r="236" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B236" s="1"/>
@@ -3292,10 +4153,9 @@
       <c r="E245" s="4"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B246" s="8"/>
-      <c r="C246" s="7"/>
-      <c r="D246" s="6"/>
-      <c r="E246" s="7"/>
+      <c r="B246" s="3"/>
+      <c r="C246" s="6"/>
+      <c r="E246" s="6"/>
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B249" s="1"/>
@@ -3358,10 +4218,9 @@
       <c r="E258" s="4"/>
     </row>
     <row r="259" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B259" s="8"/>
-      <c r="C259" s="7"/>
-      <c r="D259" s="6"/>
-      <c r="E259" s="7"/>
+      <c r="B259" s="3"/>
+      <c r="C259" s="6"/>
+      <c r="E259" s="6"/>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B262" s="1"/>
@@ -3424,10 +4283,9 @@
       <c r="E271" s="4"/>
     </row>
     <row r="272" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B272" s="8"/>
-      <c r="C272" s="7"/>
-      <c r="D272" s="6"/>
-      <c r="E272" s="7"/>
+      <c r="B272" s="3"/>
+      <c r="C272" s="6"/>
+      <c r="E272" s="6"/>
     </row>
   </sheetData>
   <scenarios current="74" show="59" sqref="G2:G11">
@@ -4174,10 +5032,11 @@
     <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4187,7 +5046,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4196,66 +5058,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>

</xml_diff>